<commit_message>
updated the bom and datasheets
</commit_message>
<xml_diff>
--- a/hardware/BOM/BOM.xlsx
+++ b/hardware/BOM/BOM.xlsx
@@ -4,10 +4,13 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650" tabRatio="477"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="PCB" sheetId="3" r:id="rId1"/>
+    <sheet name="External" sheetId="4" r:id="rId2"/>
+    <sheet name="Vendors and others" sheetId="2" r:id="rId3"/>
+    <sheet name="Component recommendations" sheetId="1" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -19,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="277" uniqueCount="162">
   <si>
     <t>Component</t>
   </si>
@@ -91,13 +94,427 @@
   </si>
   <si>
     <t>Recommendation: Flat top catridge so that it fits in the normal housings</t>
+  </si>
+  <si>
+    <t>Additional</t>
+  </si>
+  <si>
+    <t>Vendors</t>
+  </si>
+  <si>
+    <t>LCSC</t>
+  </si>
+  <si>
+    <t>JLCPCB</t>
+  </si>
+  <si>
+    <t>EasyEDA</t>
+  </si>
+  <si>
+    <t>DigiKey</t>
+  </si>
+  <si>
+    <t>Mouser</t>
+  </si>
+  <si>
+    <t>Components Data, footprints and 3D models</t>
+  </si>
+  <si>
+    <t>SnapEDA</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>This is the physical device installed on the water pipe</t>
+  </si>
+  <si>
+    <t>DigiKey [https://www.digikey.com/en/products/detail/adafruit-industries-llc/997/6827136?s=N4IgTCBcDaIIwHowB0QAIAKAbAhgZwBcBLAYzQHUcCBTAJzQGUB7LagOyaIBM0A1HLADdqIALoBfIA]</t>
+  </si>
+  <si>
+    <t>Solenoid Valve, V1</t>
+  </si>
+  <si>
+    <t>Manufacturer Part Number</t>
+  </si>
+  <si>
+    <t>Find at      (Supplier + URL)</t>
+  </si>
+  <si>
+    <t>Manufacturer</t>
+  </si>
+  <si>
+    <t>Package / Footprint</t>
+  </si>
+  <si>
+    <t>Adafruit Industries LLC</t>
+  </si>
+  <si>
+    <t>Suppiler Part Number</t>
+  </si>
+  <si>
+    <t>1528-2003-ND</t>
+  </si>
+  <si>
+    <t>This is used to switch the 12V power for the valve using the 5V logic signal</t>
+  </si>
+  <si>
+    <t>Price (USD)</t>
+  </si>
+  <si>
+    <t>Songle Relay</t>
+  </si>
+  <si>
+    <t>SRD-05VDC-SL-C</t>
+  </si>
+  <si>
+    <t>C35449</t>
+  </si>
+  <si>
+    <t>LCSC [https://www.lcsc.com/product-detail/C35449.html?s_z=n_songle%2520relay%2520%2520C37482]</t>
+  </si>
+  <si>
+    <t>Relay (PCB Switch)</t>
+  </si>
+  <si>
+    <t>This is the specific component that fits the standard "Blue sugar cube" footprint, through hole</t>
+  </si>
+  <si>
+    <t>RELAY-TH_SRD-05VDC or Relay_SPDT_Songle_SRD</t>
+  </si>
+  <si>
+    <t>Terminal Block (Valve connection)</t>
+  </si>
+  <si>
+    <t>This is the connector where the wires from the 12V Valve will screw into the PCB.</t>
+  </si>
+  <si>
+    <t>Cixi Kefa Elec</t>
+  </si>
+  <si>
+    <t>KF301-5.0-2P</t>
+  </si>
+  <si>
+    <t>C474881</t>
+  </si>
+  <si>
+    <t>LCSC [https://www.lcsc.com/product-detail/C474881.html?s_z=n_KF301-2P%2520%28C2336%29]</t>
+  </si>
+  <si>
+    <t>Turbidity sensor, S1</t>
+  </si>
+  <si>
+    <t>DFRobot</t>
+  </si>
+  <si>
+    <t>SEN0189</t>
+  </si>
+  <si>
+    <t>GRAVITY: ANALOG TURBIDITY SENSOR</t>
+  </si>
+  <si>
+    <t>DigiKey [https://www.digikey.com/en/products/detail/dfrobot/SEN0189/6588606?s=N4IgTCBcDaIMoFEByAGAjADgJwgLoF8g]</t>
+  </si>
+  <si>
+    <t>1738-1185-ND</t>
+  </si>
+  <si>
+    <t>CONN-TH_3P-P2.54_XH</t>
+  </si>
+  <si>
+    <t>Turbidity sensor (PCB connector)</t>
+  </si>
+  <si>
+    <t> 3-pin header to connect the wire coming from the sensor</t>
+  </si>
+  <si>
+    <t>hanxia</t>
+  </si>
+  <si>
+    <t>HX-XH2.54-3PZZ</t>
+  </si>
+  <si>
+    <t>LCSC [https://www.lcsc.com/product-detail/C42391661.html?s_z=n_pin%2520header]</t>
+  </si>
+  <si>
+    <t>C42391661</t>
+  </si>
+  <si>
+    <t>12 V DC Diaphragm pump, P1</t>
+  </si>
+  <si>
+    <t>This pump draws water from the source and pushes it through the Sediment/Carbon filters.</t>
+  </si>
+  <si>
+    <t>SFDP1-011-070-21</t>
+  </si>
+  <si>
+    <t>Seaflo</t>
+  </si>
+  <si>
+    <t>Amazon [https://www.amazon.com/SEAFLO-Diaphragm-Water-Pressure-Pump/dp/B0DVTJ1FKP]</t>
+  </si>
+  <si>
+    <t>CONN-TH_2P-P5.00</t>
+  </si>
+  <si>
+    <t>This is used to switch the 12V power for the pump, P1 using the 5V logic signal</t>
+  </si>
+  <si>
+    <t>Pressure sensor, S2</t>
+  </si>
+  <si>
+    <t>SEN0257</t>
+  </si>
+  <si>
+    <t>1738-1377-ND</t>
+  </si>
+  <si>
+    <t>Pressure Sensor 232.06PSI (1600kPa) Gauge 0.5 V ~ 4.5 V Cylinder, Metal</t>
+  </si>
+  <si>
+    <t>DigiKey [https://www.digikey.com/en/products/detail/dfrobot/SEN0257/8341836?s=N4IgTCBcDaIOYCcCGA3AlgFwJ4AIDuSGApgjgA4JEDOVArpTlUQHZUD2CIAugL5A]</t>
+  </si>
+  <si>
+    <t>Pressure sensor (PCB connector)</t>
+  </si>
+  <si>
+    <t>Water Flow sensor, S3</t>
+  </si>
+  <si>
+    <t>Liquid Flow Sensor 1 ~ 30 LPM 0.787" (20mm) Plastic</t>
+  </si>
+  <si>
+    <t>SEN0217</t>
+  </si>
+  <si>
+    <t>DigiKey [https://www.digikey.com/en/products/detail/dfrobot/SEN0217/6579446?s=N4IgTCBcDaIM4FMB2AGMBGA7CAugXyA]</t>
+  </si>
+  <si>
+    <t>SEN0217-ND</t>
+  </si>
+  <si>
+    <t>Color sensor, S4</t>
+  </si>
+  <si>
+    <t>TCS34725 Color Sensor Gravity Platform Evaluation Expansion Board</t>
+  </si>
+  <si>
+    <t>SEN0212</t>
+  </si>
+  <si>
+    <t>DigiKey [https://www.digikey.com/en/products/detail/dfrobot/SEN0212/7087188?s=N4IgTCBcDaIMoFEByAGMBGCBdAvkA]</t>
+  </si>
+  <si>
+    <t>1738-1291-ND</t>
+  </si>
+  <si>
+    <t>Color sensor (PCB connector)</t>
+  </si>
+  <si>
+    <t>Pin Header 4 Position 2.54mm Pitch Single Row Through Hole -40℃~+105℃</t>
+  </si>
+  <si>
+    <t>Ckmtw</t>
+  </si>
+  <si>
+    <t>B-2100S04P-A110</t>
+  </si>
+  <si>
+    <t>LCSC [https://www.lcsc.com/product-detail/C124378.html]</t>
+  </si>
+  <si>
+    <t>C124378</t>
+  </si>
+  <si>
+    <t>HDR-M-2.54_1x4</t>
+  </si>
+  <si>
+    <t>12 Watt Stainless Steel UV Sterilizer with 12V ballast [DC not AC]</t>
+  </si>
+  <si>
+    <t>https://purewater4life.co.za/12-watt-stainless-steel-uv-sterilizer-with-12v-ballast/</t>
+  </si>
+  <si>
+    <t>* SSE-012 EB-G16-12V UV Sterilizer</t>
+  </si>
+  <si>
+    <t>*UV Lamp</t>
+  </si>
+  <si>
+    <t>* UV Lamp</t>
+  </si>
+  <si>
+    <t>ALT</t>
+  </si>
+  <si>
+    <t>12VDC 1gpm 12W Fostream UV Water Steriliser UVC Lamp Ultraviolet Sterilizer</t>
+  </si>
+  <si>
+    <t>SSE-012</t>
+  </si>
+  <si>
+    <t>Agua Topone</t>
+  </si>
+  <si>
+    <t>https://aguatopone686.en.made-in-china.com/product/cxbRZNGdnAWl/China-12VDC-1gpm-12W-Fostream-UV-Water-Steriliser-UVC-Lamp-Ultraviolet-Sterilizer.html</t>
+  </si>
+  <si>
+    <t>This is used to switch the DC UV lamp using the 5V logic signal</t>
+  </si>
+  <si>
+    <t>Terminal Block (Pump connection)</t>
+  </si>
+  <si>
+    <t>Terminal Block (UV lamp connection)</t>
+  </si>
+  <si>
+    <t>Water Level sensor, S5</t>
+  </si>
+  <si>
+    <t>WEATHER-PROOF ULTRASONIC SENSOR</t>
+  </si>
+  <si>
+    <t>SEN0208</t>
+  </si>
+  <si>
+    <t>DigiKey [https://www.digikey.com/en/products/detail/dfrobot/SEN0208/6588472]</t>
+  </si>
+  <si>
+    <t>1738-1050-ND</t>
+  </si>
+  <si>
+    <t>Water Level sensor (PCB connector)</t>
+  </si>
+  <si>
+    <t>Connector Header 4 position 2.5mm Pitch 3A Right Angle -25℃~+85℃</t>
+  </si>
+  <si>
+    <t>Bossie</t>
+  </si>
+  <si>
+    <t>BX-XH2.54-4PWZ</t>
+  </si>
+  <si>
+    <t>LCSC [https://www.lcsc.com/product-detail/C18077844.html?s_z=n_XH2.54-4P%2520White%2520Box%2520Header]</t>
+  </si>
+  <si>
+    <t>C18077844</t>
+  </si>
+  <si>
+    <t>TDS sensor, S6</t>
+  </si>
+  <si>
+    <t>GRAVITY ANALOG TDS SENSOR/METER</t>
+  </si>
+  <si>
+    <t>SEN0244</t>
+  </si>
+  <si>
+    <t>DigiKey [https://www.digikey.com/en/products/detail/dfrobot/SEN0244/8019062?s=N4IgTCBcDaIMoFEByAGMAWdIC6BfIA]</t>
+  </si>
+  <si>
+    <t>1738-1368-ND</t>
+  </si>
+  <si>
+    <t>TDS sensor (PCB connector)</t>
+  </si>
+  <si>
+    <t>Connector Header 3 position 2.54mm Pitch 3A Through Hole -25℃~+85℃</t>
+  </si>
+  <si>
+    <t>LCSC [https://www.lcsc.com/product-detail/C42391661.html]</t>
+  </si>
+  <si>
+    <t>PH sensor, S7</t>
+  </si>
+  <si>
+    <t>GRAVITY: ANALOG PH SENSOR/METER</t>
+  </si>
+  <si>
+    <t>SEN0161-V2</t>
+  </si>
+  <si>
+    <t>DigiKey [https://www.digikey.com/en/products/detail/dfrobot/SEN0161-V2/9608223?s=N4IgTCBcDaIMoFEByAGAjANjQWgGoQF0BfIA]</t>
+  </si>
+  <si>
+    <t>SEN0161-V2-ND</t>
+  </si>
+  <si>
+    <t>Relay, Re1</t>
+  </si>
+  <si>
+    <t>Relay, Re2</t>
+  </si>
+  <si>
+    <t>Relay, Re3</t>
+  </si>
+  <si>
+    <t>Relay, Re4</t>
+  </si>
+  <si>
+    <t>This is used to switch the 12V power for the pump, P2 using the 5V logic signal</t>
+  </si>
+  <si>
+    <t>12 V DC Diaphragm pump, P2</t>
+  </si>
+  <si>
+    <t>Pressure sensor, S8</t>
+  </si>
+  <si>
+    <t>Solenoid Valve, V2</t>
+  </si>
+  <si>
+    <t>Relay, Re5</t>
+  </si>
+  <si>
+    <t>Microcontroller</t>
+  </si>
+  <si>
+    <t>Espressif Systems</t>
+  </si>
+  <si>
+    <t>ESP32-WROOM-32E</t>
+  </si>
+  <si>
+    <t>Voltage regulator</t>
+  </si>
+  <si>
+    <t>UMW</t>
+  </si>
+  <si>
+    <t>AMS1117-3.3</t>
+  </si>
+  <si>
+    <t>Linear Voltage Regulator IC Positive Fixed 1 Output 1A SOT-223-3L</t>
+  </si>
+  <si>
+    <t>DigiKey [https://www.digikey.com/en/products/detail/umw/AMS1117-3-3/17635254]</t>
+  </si>
+  <si>
+    <t>4518-AMS1117-3.3TR-ND</t>
+  </si>
+  <si>
+    <t>SOT-223</t>
+  </si>
+  <si>
+    <t>Bluetooth, WiFi 802.11b/g/n, Bluetooth v4.2 +EDR, Class 1, 2 and 3 Transceiver Module 2.4GHz ~ 2.5GHz Integrated, Trace Surface Mount</t>
+  </si>
+  <si>
+    <t>ESP32-WROOM-32E-N4</t>
+  </si>
+  <si>
+    <t>DigiKey [https://www.digikey.com/en/products/detail/espressif-systems/ESP32-WROOM-32E-N4/11613148]</t>
+  </si>
+  <si>
+    <t>1965-ESP32-WROOM-32E-N4TR-ND</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -111,16 +528,101 @@
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="14">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59996337778862885"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59996337778862885"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59996337778862885"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14996795556505021"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59996337778862885"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39994506668294322"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39994506668294322"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -128,19 +630,143 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="61">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFCCFF66"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -415,22 +1041,1244 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C16"/>
+  <dimension ref="A1:I49"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A35" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E55" sqref="E55"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="20.1796875" style="16" customWidth="1"/>
+    <col min="2" max="2" width="5.7265625" style="17" customWidth="1"/>
+    <col min="3" max="4" width="16.453125" style="17" customWidth="1"/>
+    <col min="5" max="5" width="18.36328125" style="17" customWidth="1"/>
+    <col min="6" max="6" width="12.90625" style="17" customWidth="1"/>
+    <col min="7" max="7" width="9.26953125" style="17" customWidth="1"/>
+    <col min="8" max="8" width="10.1796875" style="17" customWidth="1"/>
+    <col min="9" max="9" width="12.7265625" style="17" customWidth="1"/>
+    <col min="10" max="16384" width="8.7265625" style="17"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" s="3" customFormat="1" ht="36.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" s="3" customFormat="1" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="2"/>
+    </row>
+    <row r="3" spans="1:9" s="3" customFormat="1" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="B3" s="3">
+        <v>1</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>159</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="G3" s="3">
+        <v>4.84</v>
+      </c>
+      <c r="H3" s="60" t="s">
+        <v>160</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" s="3" customFormat="1" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="B4" s="3">
+        <v>1</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="G4" s="3">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" s="3" customFormat="1" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="2"/>
+    </row>
+    <row r="6" spans="1:9" s="3" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="2"/>
+    </row>
+    <row r="7" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="25" t="s">
+        <v>139</v>
+      </c>
+      <c r="B7" s="26"/>
+      <c r="C7" s="26" t="s">
+        <v>44</v>
+      </c>
+      <c r="D7" s="26"/>
+      <c r="E7" s="26"/>
+      <c r="F7" s="26"/>
+      <c r="G7" s="26"/>
+      <c r="H7" s="26"/>
+    </row>
+    <row r="8" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="B8" s="6">
+        <v>1</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="E8" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="F8" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="G8" s="6">
+        <v>1.48</v>
+      </c>
+      <c r="H8" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="I8" s="6" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="B9" s="6">
+        <v>1</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="E9" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="F9" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="G9" s="6">
+        <v>0.44</v>
+      </c>
+      <c r="H9" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="I9" s="6" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="5"/>
+    </row>
+    <row r="12" spans="1:9" s="8" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="B12" s="8">
+        <v>1</v>
+      </c>
+      <c r="C12" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="D12" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="E12" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="F12" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="G12" s="8">
+        <v>0.05</v>
+      </c>
+      <c r="H12" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="I12" s="8" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="14" spans="1:9" s="10" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="9"/>
+    </row>
+    <row r="15" spans="1:9" s="11" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="27" t="s">
+        <v>140</v>
+      </c>
+      <c r="B15" s="28"/>
+      <c r="C15" s="28" t="s">
+        <v>78</v>
+      </c>
+      <c r="D15" s="28"/>
+      <c r="E15" s="28"/>
+      <c r="F15" s="28"/>
+      <c r="G15" s="28"/>
+      <c r="H15" s="28"/>
+    </row>
+    <row r="16" spans="1:9" s="10" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="B16" s="10">
+        <v>1</v>
+      </c>
+      <c r="C16" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="D16" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="E16" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="F16" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="G16" s="10">
+        <v>1.48</v>
+      </c>
+      <c r="H16" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="I16" s="10" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" s="10" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="9" t="s">
+        <v>113</v>
+      </c>
+      <c r="B17" s="10">
+        <v>1</v>
+      </c>
+      <c r="C17" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="D17" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="E17" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="F17" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="G17" s="10">
+        <v>0.44</v>
+      </c>
+      <c r="H17" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="I17" s="10" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" s="10" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="9"/>
+    </row>
+    <row r="20" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="12" t="s">
+        <v>84</v>
+      </c>
+      <c r="B20" s="13">
+        <v>1</v>
+      </c>
+      <c r="C20" s="13" t="s">
+        <v>67</v>
+      </c>
+      <c r="D20" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="E20" s="13" t="s">
+        <v>69</v>
+      </c>
+      <c r="F20" s="13" t="s">
+        <v>65</v>
+      </c>
+      <c r="G20" s="13">
+        <v>0.05</v>
+      </c>
+      <c r="H20" s="13" t="s">
+        <v>70</v>
+      </c>
+      <c r="I20" s="13" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" s="15" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A22" s="14" t="s">
+        <v>84</v>
+      </c>
+      <c r="B22" s="15">
+        <v>1</v>
+      </c>
+      <c r="C22" s="15" t="s">
+        <v>67</v>
+      </c>
+      <c r="D22" s="15" t="s">
+        <v>68</v>
+      </c>
+      <c r="E22" s="15" t="s">
+        <v>69</v>
+      </c>
+      <c r="F22" s="15" t="s">
+        <v>65</v>
+      </c>
+      <c r="G22" s="15">
+        <v>0.05</v>
+      </c>
+      <c r="H22" s="15" t="s">
+        <v>70</v>
+      </c>
+      <c r="I22" s="15" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A24" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="B24" s="6">
+        <v>1</v>
+      </c>
+      <c r="C24" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="D24" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="E24" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="F24" s="24" t="s">
+        <v>101</v>
+      </c>
+      <c r="G24" s="6">
+        <v>0.48</v>
+      </c>
+      <c r="H24" s="6" t="s">
+        <v>99</v>
+      </c>
+      <c r="I24" s="6" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" s="31" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A26" s="29" t="s">
+        <v>141</v>
+      </c>
+      <c r="B26" s="30"/>
+      <c r="C26" s="30" t="s">
+        <v>112</v>
+      </c>
+      <c r="D26" s="30"/>
+      <c r="E26" s="30"/>
+      <c r="F26" s="30"/>
+      <c r="G26" s="30"/>
+      <c r="H26" s="30"/>
+    </row>
+    <row r="27" spans="1:9" s="33" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A27" s="32" t="s">
+        <v>50</v>
+      </c>
+      <c r="B27" s="33">
+        <v>1</v>
+      </c>
+      <c r="C27" s="33" t="s">
+        <v>51</v>
+      </c>
+      <c r="D27" s="33" t="s">
+        <v>46</v>
+      </c>
+      <c r="E27" s="33" t="s">
+        <v>47</v>
+      </c>
+      <c r="F27" s="33" t="s">
+        <v>52</v>
+      </c>
+      <c r="G27" s="33">
+        <v>1.48</v>
+      </c>
+      <c r="H27" s="33" t="s">
+        <v>49</v>
+      </c>
+      <c r="I27" s="33" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" s="33" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A28" s="32" t="s">
+        <v>114</v>
+      </c>
+      <c r="B28" s="33">
+        <v>1</v>
+      </c>
+      <c r="C28" s="33" t="s">
+        <v>54</v>
+      </c>
+      <c r="D28" s="33" t="s">
+        <v>55</v>
+      </c>
+      <c r="E28" s="33" t="s">
+        <v>56</v>
+      </c>
+      <c r="F28" s="33" t="s">
+        <v>77</v>
+      </c>
+      <c r="G28" s="33">
+        <v>0.44</v>
+      </c>
+      <c r="H28" s="33" t="s">
+        <v>58</v>
+      </c>
+      <c r="I28" s="33" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" s="37" customFormat="1" ht="12.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A30" s="36" t="s">
+        <v>120</v>
+      </c>
+      <c r="B30" s="37">
+        <v>1</v>
+      </c>
+      <c r="C30" s="37" t="s">
+        <v>121</v>
+      </c>
+      <c r="D30" s="37" t="s">
+        <v>122</v>
+      </c>
+      <c r="E30" s="37" t="s">
+        <v>123</v>
+      </c>
+      <c r="G30" s="37">
+        <v>0.4</v>
+      </c>
+      <c r="H30" s="37" t="s">
+        <v>124</v>
+      </c>
+      <c r="I30" s="37" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" s="40" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A32" s="39" t="s">
+        <v>131</v>
+      </c>
+      <c r="B32" s="40">
+        <v>1</v>
+      </c>
+      <c r="C32" s="40" t="s">
+        <v>132</v>
+      </c>
+      <c r="D32" s="40" t="s">
+        <v>68</v>
+      </c>
+      <c r="E32" s="40" t="s">
+        <v>69</v>
+      </c>
+      <c r="G32" s="40">
+        <v>0.05</v>
+      </c>
+      <c r="H32" s="40" t="s">
+        <v>133</v>
+      </c>
+      <c r="I32" s="40" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" s="43" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A34" s="42" t="s">
+        <v>131</v>
+      </c>
+      <c r="B34" s="43">
+        <v>1</v>
+      </c>
+      <c r="C34" s="43" t="s">
+        <v>132</v>
+      </c>
+      <c r="D34" s="43" t="s">
+        <v>68</v>
+      </c>
+      <c r="E34" s="43" t="s">
+        <v>69</v>
+      </c>
+      <c r="G34" s="43">
+        <v>0.05</v>
+      </c>
+      <c r="H34" s="43" t="s">
+        <v>133</v>
+      </c>
+      <c r="I34" s="43" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" s="46" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A36" s="45"/>
+    </row>
+    <row r="37" spans="1:9" s="49" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A37" s="47" t="s">
+        <v>142</v>
+      </c>
+      <c r="B37" s="48"/>
+      <c r="C37" s="48" t="s">
+        <v>143</v>
+      </c>
+      <c r="D37" s="48"/>
+      <c r="E37" s="48"/>
+      <c r="F37" s="48"/>
+      <c r="G37" s="48"/>
+      <c r="H37" s="48"/>
+    </row>
+    <row r="38" spans="1:9" s="46" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A38" s="45" t="s">
+        <v>50</v>
+      </c>
+      <c r="B38" s="46">
+        <v>1</v>
+      </c>
+      <c r="C38" s="46" t="s">
+        <v>51</v>
+      </c>
+      <c r="D38" s="46" t="s">
+        <v>46</v>
+      </c>
+      <c r="E38" s="46" t="s">
+        <v>47</v>
+      </c>
+      <c r="F38" s="46" t="s">
+        <v>52</v>
+      </c>
+      <c r="G38" s="46">
+        <v>1.48</v>
+      </c>
+      <c r="H38" s="46" t="s">
+        <v>49</v>
+      </c>
+      <c r="I38" s="46" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" s="46" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A39" s="45" t="s">
+        <v>113</v>
+      </c>
+      <c r="B39" s="46">
+        <v>1</v>
+      </c>
+      <c r="C39" s="46" t="s">
+        <v>54</v>
+      </c>
+      <c r="D39" s="46" t="s">
+        <v>55</v>
+      </c>
+      <c r="E39" s="46" t="s">
+        <v>56</v>
+      </c>
+      <c r="F39" s="46" t="s">
+        <v>77</v>
+      </c>
+      <c r="G39" s="46">
+        <v>0.44</v>
+      </c>
+      <c r="H39" s="46" t="s">
+        <v>58</v>
+      </c>
+      <c r="I39" s="46" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" s="46" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A40" s="45"/>
+    </row>
+    <row r="42" spans="1:9" s="53" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A42" s="52" t="s">
+        <v>84</v>
+      </c>
+      <c r="B42" s="53">
+        <v>1</v>
+      </c>
+      <c r="C42" s="53" t="s">
+        <v>67</v>
+      </c>
+      <c r="D42" s="53" t="s">
+        <v>68</v>
+      </c>
+      <c r="E42" s="53" t="s">
+        <v>69</v>
+      </c>
+      <c r="F42" s="53" t="s">
+        <v>65</v>
+      </c>
+      <c r="G42" s="53">
+        <v>0.05</v>
+      </c>
+      <c r="H42" s="53" t="s">
+        <v>70</v>
+      </c>
+      <c r="I42" s="53" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" s="57" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A44" s="55" t="s">
+        <v>147</v>
+      </c>
+      <c r="B44" s="56"/>
+      <c r="C44" s="56" t="s">
+        <v>44</v>
+      </c>
+      <c r="D44" s="56"/>
+      <c r="E44" s="56"/>
+      <c r="F44" s="56"/>
+      <c r="G44" s="56"/>
+      <c r="H44" s="56"/>
+    </row>
+    <row r="45" spans="1:9" s="59" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A45" s="58" t="s">
+        <v>50</v>
+      </c>
+      <c r="B45" s="59">
+        <v>1</v>
+      </c>
+      <c r="C45" s="59" t="s">
+        <v>51</v>
+      </c>
+      <c r="D45" s="59" t="s">
+        <v>46</v>
+      </c>
+      <c r="E45" s="59" t="s">
+        <v>47</v>
+      </c>
+      <c r="F45" s="59" t="s">
+        <v>52</v>
+      </c>
+      <c r="G45" s="59">
+        <v>1.48</v>
+      </c>
+      <c r="H45" s="59" t="s">
+        <v>49</v>
+      </c>
+      <c r="I45" s="59" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" s="59" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A46" s="58" t="s">
+        <v>53</v>
+      </c>
+      <c r="B46" s="59">
+        <v>1</v>
+      </c>
+      <c r="C46" s="59" t="s">
+        <v>54</v>
+      </c>
+      <c r="D46" s="59" t="s">
+        <v>55</v>
+      </c>
+      <c r="E46" s="59" t="s">
+        <v>56</v>
+      </c>
+      <c r="F46" s="59" t="s">
+        <v>77</v>
+      </c>
+      <c r="G46" s="59">
+        <v>0.44</v>
+      </c>
+      <c r="H46" s="59" t="s">
+        <v>58</v>
+      </c>
+      <c r="I46" s="59" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" s="59" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A47" s="58"/>
+    </row>
+    <row r="49" spans="7:7" x14ac:dyDescent="0.35">
+      <c r="G49" s="17">
+        <f>SUM(G3:G47)</f>
+        <v>15.910000000000004</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="10">
+    <mergeCell ref="A37:B37"/>
+    <mergeCell ref="C37:H37"/>
+    <mergeCell ref="A44:B44"/>
+    <mergeCell ref="C44:H44"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="C7:H7"/>
+    <mergeCell ref="A15:B15"/>
+    <mergeCell ref="C15:H15"/>
+    <mergeCell ref="A26:B26"/>
+    <mergeCell ref="C26:H26"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I30"/>
+  <sheetViews>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G30" sqref="G30"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="16.7265625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="5.6328125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="27" style="1" customWidth="1"/>
+    <col min="4" max="4" width="19.26953125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="13.6328125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="10.1796875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="8.7265625" style="1"/>
+    <col min="8" max="8" width="14.7265625" style="1" customWidth="1"/>
+    <col min="9" max="9" width="14.453125" style="1" customWidth="1"/>
+    <col min="10" max="16384" width="8.7265625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" s="18" customFormat="1" ht="62" x14ac:dyDescent="0.35">
+      <c r="A1" s="18" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="D1" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="E1" s="18" t="s">
+        <v>37</v>
+      </c>
+      <c r="F1" s="18" t="s">
+        <v>40</v>
+      </c>
+      <c r="G1" s="18" t="s">
+        <v>45</v>
+      </c>
+      <c r="H1" s="18" t="s">
+        <v>38</v>
+      </c>
+      <c r="I1" s="18" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="3" spans="1:9" s="19" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="B3" s="19">
+        <v>1</v>
+      </c>
+      <c r="C3" s="19" t="s">
+        <v>34</v>
+      </c>
+      <c r="D3" s="19" t="s">
+        <v>41</v>
+      </c>
+      <c r="G3" s="19">
+        <v>6.95</v>
+      </c>
+      <c r="H3" s="19" t="s">
+        <v>35</v>
+      </c>
+      <c r="I3" s="19" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" s="20" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="20" t="s">
+        <v>59</v>
+      </c>
+      <c r="B5" s="20">
+        <v>1</v>
+      </c>
+      <c r="C5" s="20" t="s">
+        <v>62</v>
+      </c>
+      <c r="D5" s="20" t="s">
+        <v>60</v>
+      </c>
+      <c r="E5" s="20" t="s">
+        <v>61</v>
+      </c>
+      <c r="G5" s="20">
+        <v>9.9</v>
+      </c>
+      <c r="H5" s="20" t="s">
+        <v>63</v>
+      </c>
+      <c r="I5" s="20" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" s="21" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="21" t="s">
+        <v>72</v>
+      </c>
+      <c r="B7" s="21">
+        <v>1</v>
+      </c>
+      <c r="C7" s="21" t="s">
+        <v>73</v>
+      </c>
+      <c r="D7" s="21" t="s">
+        <v>75</v>
+      </c>
+      <c r="E7" s="21" t="s">
+        <v>74</v>
+      </c>
+      <c r="G7" s="21">
+        <v>34</v>
+      </c>
+      <c r="H7" s="21" t="s">
+        <v>76</v>
+      </c>
+      <c r="I7" s="21">
+        <v>810039497982</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" s="22" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="22" t="s">
+        <v>79</v>
+      </c>
+      <c r="B9" s="22">
+        <v>1</v>
+      </c>
+      <c r="C9" s="22" t="s">
+        <v>82</v>
+      </c>
+      <c r="D9" s="22" t="s">
+        <v>60</v>
+      </c>
+      <c r="E9" s="22" t="s">
+        <v>80</v>
+      </c>
+      <c r="G9" s="22">
+        <v>17.5</v>
+      </c>
+      <c r="H9" s="22" t="s">
+        <v>83</v>
+      </c>
+      <c r="I9" s="22" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" s="23" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="23" t="s">
+        <v>85</v>
+      </c>
+      <c r="B11" s="23">
+        <v>1</v>
+      </c>
+      <c r="C11" s="23" t="s">
+        <v>86</v>
+      </c>
+      <c r="D11" s="23" t="s">
+        <v>60</v>
+      </c>
+      <c r="E11" s="23" t="s">
+        <v>87</v>
+      </c>
+      <c r="G11" s="23">
+        <v>8.99</v>
+      </c>
+      <c r="H11" s="23" t="s">
+        <v>88</v>
+      </c>
+      <c r="I11" s="23" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" s="19" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="19" t="s">
+        <v>90</v>
+      </c>
+      <c r="B13" s="19">
+        <v>1</v>
+      </c>
+      <c r="C13" s="19" t="s">
+        <v>91</v>
+      </c>
+      <c r="D13" s="19" t="s">
+        <v>60</v>
+      </c>
+      <c r="E13" s="19" t="s">
+        <v>92</v>
+      </c>
+      <c r="G13" s="19">
+        <v>7.9</v>
+      </c>
+      <c r="H13" s="19" t="s">
+        <v>93</v>
+      </c>
+      <c r="I13" s="19" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" s="34" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="34" t="s">
+        <v>105</v>
+      </c>
+      <c r="B15" s="34">
+        <v>1</v>
+      </c>
+      <c r="C15" s="34" t="s">
+        <v>102</v>
+      </c>
+      <c r="E15" s="34" t="s">
+        <v>104</v>
+      </c>
+      <c r="G15" s="34">
+        <v>70</v>
+      </c>
+      <c r="H15" s="35" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" s="34" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="34" t="s">
+        <v>106</v>
+      </c>
+      <c r="B16" s="34" t="s">
+        <v>107</v>
+      </c>
+      <c r="C16" s="34" t="s">
+        <v>108</v>
+      </c>
+      <c r="D16" s="34" t="s">
+        <v>110</v>
+      </c>
+      <c r="E16" s="34" t="s">
+        <v>109</v>
+      </c>
+      <c r="G16" s="34">
+        <v>18</v>
+      </c>
+      <c r="H16" s="35" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" s="38" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="38" t="s">
+        <v>115</v>
+      </c>
+      <c r="B18" s="38">
+        <v>1</v>
+      </c>
+      <c r="C18" s="38" t="s">
+        <v>116</v>
+      </c>
+      <c r="D18" s="38" t="s">
+        <v>60</v>
+      </c>
+      <c r="E18" s="38" t="s">
+        <v>117</v>
+      </c>
+      <c r="G18" s="38">
+        <v>16</v>
+      </c>
+      <c r="H18" s="38" t="s">
+        <v>118</v>
+      </c>
+      <c r="I18" s="38" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" s="41" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="41" t="s">
+        <v>126</v>
+      </c>
+      <c r="B20" s="41">
+        <v>1</v>
+      </c>
+      <c r="C20" s="41" t="s">
+        <v>127</v>
+      </c>
+      <c r="D20" s="41" t="s">
+        <v>60</v>
+      </c>
+      <c r="E20" s="41" t="s">
+        <v>128</v>
+      </c>
+      <c r="G20" s="41">
+        <v>11.8</v>
+      </c>
+      <c r="H20" s="41" t="s">
+        <v>129</v>
+      </c>
+      <c r="I20" s="41" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" s="44" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A22" s="44" t="s">
+        <v>134</v>
+      </c>
+      <c r="B22" s="44">
+        <v>1</v>
+      </c>
+      <c r="C22" s="44" t="s">
+        <v>135</v>
+      </c>
+      <c r="D22" s="44" t="s">
+        <v>60</v>
+      </c>
+      <c r="E22" s="44" t="s">
+        <v>136</v>
+      </c>
+      <c r="G22" s="44">
+        <v>39.5</v>
+      </c>
+      <c r="H22" s="44" t="s">
+        <v>137</v>
+      </c>
+      <c r="I22" s="44" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" s="50" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A24" s="50" t="s">
+        <v>144</v>
+      </c>
+      <c r="B24" s="50">
+        <v>1</v>
+      </c>
+      <c r="C24" s="50" t="s">
+        <v>73</v>
+      </c>
+      <c r="D24" s="50" t="s">
+        <v>75</v>
+      </c>
+      <c r="E24" s="50" t="s">
+        <v>74</v>
+      </c>
+      <c r="G24" s="50">
+        <v>34</v>
+      </c>
+      <c r="H24" s="50" t="s">
+        <v>76</v>
+      </c>
+      <c r="I24" s="50">
+        <v>810039497982</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" s="51" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A26" s="51" t="s">
+        <v>145</v>
+      </c>
+      <c r="B26" s="51">
+        <v>1</v>
+      </c>
+      <c r="C26" s="51" t="s">
+        <v>82</v>
+      </c>
+      <c r="D26" s="51" t="s">
+        <v>60</v>
+      </c>
+      <c r="E26" s="51" t="s">
+        <v>80</v>
+      </c>
+      <c r="G26" s="51">
+        <v>17.5</v>
+      </c>
+      <c r="H26" s="51" t="s">
+        <v>83</v>
+      </c>
+      <c r="I26" s="51" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" s="54" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A28" s="54" t="s">
+        <v>146</v>
+      </c>
+      <c r="B28" s="54">
+        <v>1</v>
+      </c>
+      <c r="C28" s="54" t="s">
+        <v>34</v>
+      </c>
+      <c r="D28" s="54" t="s">
+        <v>41</v>
+      </c>
+      <c r="G28" s="54">
+        <v>6.95</v>
+      </c>
+      <c r="H28" s="54" t="s">
+        <v>35</v>
+      </c>
+      <c r="I28" s="54" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="G30" s="1">
+        <f>SUM(G3:G28)</f>
+        <v>298.99</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="H16" r:id="rId1"/>
+    <hyperlink ref="H15" r:id="rId2"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C8" sqref="C8"/>
+      <selection pane="bottomLeft" sqref="A1:XFD1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="23" customWidth="1"/>
+    <col min="2" max="2" width="31.7265625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>30</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D16"/>
+  <sheetViews>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="27.26953125" style="1" customWidth="1"/>
     <col min="2" max="2" width="6.6328125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="14.6328125" style="1" customWidth="1"/>
-    <col min="4" max="16384" width="8.7265625" style="1"/>
+    <col min="3" max="4" width="28.6328125" style="1" customWidth="1"/>
+    <col min="5" max="16384" width="8.7265625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -440,115 +2288,118 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D1" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="1">
         <v>2</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B4" s="1">
         <v>1</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="D4" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>17</v>
       </c>
       <c r="B5" s="1">
         <v>1</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="D5" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>14</v>
       </c>
       <c r="B6" s="1">
         <v>1</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="D6" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>16</v>
       </c>
       <c r="B7" s="1">
         <v>1</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="D7" s="1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
         <v>22</v>
       </c>
       <c r="B8" s="1">
         <v>1</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="D8" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
         <v>20</v>
       </c>
       <c r="B9" s="1">
         <v>5</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="D9" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B13" s="1">
         <v>1</v>
       </c>
-      <c r="C13" s="1" t="s">
+      <c r="D13" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C16" s="1" t="s">
+      <c r="D16" s="1" t="s">
         <v>11</v>
       </c>
     </row>

</xml_diff>